<commit_message>
#updates in GUI and Excel settings
</commit_message>
<xml_diff>
--- a/KeywordDriven.Desktop/TestCases.xlsx
+++ b/KeywordDriven.Desktop/TestCases.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB64995F-678C-448A-8924-3DFEE1A33C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB5A00F-7656-4A10-AD46-312F412683C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="502" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="502" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
     <sheet name="Pages Objects" sheetId="3" r:id="rId2"/>
     <sheet name="Locators" sheetId="5" r:id="rId3"/>
-    <sheet name="Test Cases" sheetId="2" r:id="rId4"/>
-    <sheet name="Test Steps" sheetId="1" r:id="rId5"/>
+    <sheet name="TestCases" sheetId="2" r:id="rId4"/>
+    <sheet name="TestSteps" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ActionKeywords">Settings!$A$2:$A$16</definedName>
@@ -41,9 +41,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="81">
   <si>
-    <t>TestCase ID</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -56,12 +53,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>Page Object</t>
-  </si>
-  <si>
     <t>Page Name</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>Open Chrome Browser</t>
   </si>
   <si>
-    <t>Step No</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -263,9 +251,6 @@
     <t>Assert doodles</t>
   </si>
   <si>
-    <t>AssetElementContains</t>
-  </si>
-  <si>
     <t>//ul[@id='archive-list']/li/div</t>
   </si>
   <si>
@@ -282,6 +267,21 @@
   </si>
   <si>
     <t>Auro</t>
+  </si>
+  <si>
+    <t>PageName</t>
+  </si>
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>StepNo</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>AssertTextPresent</t>
   </si>
 </sst>
 </file>
@@ -786,7 +786,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -800,112 +800,112 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -932,63 +932,63 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1002,7 +1002,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1014,90 +1014,90 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1110,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1126,48 +1126,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1198,152 +1198,152 @@
     <col min="4" max="4" width="13.7265625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="37.81640625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="23.81640625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="49.81640625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.90625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="10.6328125" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.08984375" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" s="12">
         <v>1</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3" s="12">
         <v>2</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="19" t="s">
         <v>65</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" s="12">
         <v>3</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B5" s="12">
         <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" s="12">
         <v>5</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B7" s="12">
         <v>6</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G7" s="14">
         <v>5</v>
@@ -1351,163 +1351,163 @@
     </row>
     <row r="8" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B8" s="17">
         <v>7</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" s="14">
         <v>1</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10" s="14">
         <v>2</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>65</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>69</v>
       </c>
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" s="14">
         <v>3</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B12" s="14">
         <v>4</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="14">
         <v>5</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B14" s="14">
         <v>6</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="F14" s="12" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B15" s="14">
         <v>7</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G15" s="14">
         <v>5</v>
@@ -1516,18 +1516,18 @@
     </row>
     <row r="16" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B16" s="17">
         <v>8</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>

</xml_diff>